<commit_message>
Murder Weapons By State: Added Barplots
</commit_message>
<xml_diff>
--- a/data/Crime_In_US_By_State/Crime_In_US_By_State_2015.xlsx
+++ b/data/Crime_In_US_By_State/Crime_In_US_By_State_2015.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19452377-C353-2D42-ACA2-D1AB0967AA8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15D4FEB-DB76-734B-9C5E-9A2264929656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5200" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="15tbl05" sheetId="4" r:id="rId1"/>
@@ -1304,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K51" sqref="A1:K51"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2458,7 +2458,7 @@
         <v>19795791</v>
       </c>
       <c r="E33" s="14">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="F33" s="14">
         <v>6074</v>

</xml_diff>